<commit_message>
Historical Data Version 1
</commit_message>
<xml_diff>
--- a/BackendSystem/HISTORYDATA.xlsx
+++ b/BackendSystem/HISTORYDATA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Solutions" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,9 @@
     <sheet name="Users" sheetId="4" r:id="rId7"/>
     <sheet name="Role ID" sheetId="7" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="bkmk_knownwin10" localSheetId="0">Solutions!$D$19</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="121">
   <si>
     <t>EDU</t>
   </si>
@@ -79,18 +82,9 @@
     <t>How to install MS Office Student Edition</t>
   </si>
   <si>
-    <t>Our university provides a MS Office Student Edition for each student. Please go to this link and follow the steps described.</t>
-  </si>
-  <si>
     <t>German student visa documents</t>
   </si>
   <si>
-    <t>Which documnets are provided by university.</t>
-  </si>
-  <si>
-    <t>All documnets could be downloaded from student university page in documents section.</t>
-  </si>
-  <si>
     <t>Ticket Text(255)</t>
   </si>
   <si>
@@ -197,13 +191,274 @@
   </si>
   <si>
     <t>ZSTSMANAG</t>
+  </si>
+  <si>
+    <t>How do I reinstall Office?</t>
+  </si>
+  <si>
+    <t>For Office 365 subscriptions: 
+We recommend you first deactivate the install you don't need anymore and then uninstall it from that PC or Mac. 
+See Deactivate an Office 365 Home, Personal, or University install. 
+Remember, with Office 365 Home, you can install Office on up to 5 PCs or Macs; with Office 365 Personal you can only install Office on 1 PC or 1 Mac; and with Office 365 University you can install on 2 PCs or Macs. Installing Office on more computers than what your plan allows will result in activation and unlicensed product errors.</t>
+  </si>
+  <si>
+    <t>Install Office on a mobile device (iOS, Android, or Windows phone or tablet)</t>
+  </si>
+  <si>
+    <t>You get a KERNEL32.dll error when trying to install Office and other system requirement issues</t>
+  </si>
+  <si>
+    <t>The Office apps for Android, iOS (iPhone or iPad), or Windows mobile devices are available to download from the app store for your device. For details on how to download the apps and set them up, select your device from below:
+Install and set up Office on an Android 
+Install and set up Office on an iPhone or iPad
+Install Office Mobile apps on a Windows 10 device or Set up Office apps on Windows Phone
+In most cases you can do basic editing on most of these devices, however if you have a qualifying Office 365 subscription, you get access to the apps extra features. See What you can do in the Office apps on an Android, iOS, or Windows mobile device with an Office 365 subscription.</t>
+  </si>
+  <si>
+    <t>If you're trying to install Office on a computer running Windows XP or Windows Vista, you may get an error that says the dynamic library KERNEL 32.dll can't be located. This occurs because Office 2016 and Office 2013 isn't supported on these versions of Windows. For more information, see Why can’t I install Office 2013 or Office 2016 on Windows XP or Windows Vista?
+If you're not sure which operating system you have, see Which Windows operating system am I running? or Find the OS X version and build number on your Mac.
+Check that your computer meets the minimum system requirements to install Office. You need a computer running Windows 7, Windows 8, or Windows 10. See System requirements for Office for a list of additional requirements.</t>
+  </si>
+  <si>
+    <t>IN-HOUSE NETWORK AT UNIVERSITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC rooms of the respective faculties; information available at the secretariat | Central library (Bonhoefferstraße 8, vis-à-vis CUBE canteen)
+Hint:
+The PC rooms except the library are mainly used by the respective faculties on their own.
+If you would like to borrow technical equipment, please ask the secretariat of you own faculty first.
+Campus web portal : matriculation number@stud.hochschule-heidelberg.de
+W-LAN (wlanfh1x, eduroam) : matriculation number@stud.hochschule-heidelberg.de
+Windows (e.g. PC pool): matriculation number@stud.hochschule-heidelberg.de
+E-mail : SRHK\matriculation number
+ILIAS : matriculation number
+Good news: The password is the same for all systems!
+Hint: For registration at further, specific systems that are used at your faculty, please contact the person in charge.
+</t>
+  </si>
+  <si>
+    <t>WHERE CAN I REGISTER? And HOW CAN I REGISTER?</t>
+  </si>
+  <si>
+    <t>PASSWORD FORGOTTEN?</t>
+  </si>
+  <si>
+    <t>Request a New Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you forgot your password you can request a new one:
+ https://campus.hochschuleheidelberg.de/
+For using this feature, your private e-mail address must always be kept up-to-date in the Campus web
+portal.
+</t>
+  </si>
+  <si>
+    <t>When are my classes?</t>
+  </si>
+  <si>
+    <t>How are the credit system and the grading?</t>
+  </si>
+  <si>
+    <t>Can I work with my student visa?</t>
+  </si>
+  <si>
+    <t>All lectures are 90 minutes long (in the German system, this counts as two 45-minute "academic hours") with a 15-minute break between each lecture.
+Generally, morning classes are set to begin at 9.30 a.m. (although some do start as early as 7.45). After a 75-minute break for lunch, afternoon classes resume at 2.00 p.m. and can take place at any time slot well into the evening. Most students only have a few lectures per day, however.
+Individual timetables will be issued through the respective faculties.</t>
+  </si>
+  <si>
+    <t>Part-time jobs and internships offer a perfect opportunity to gain some work experience in the German labor market and make useful career contacts.
+International students are only allowed to work in Germany under certain conditions. A part-time job may supplement your budget, but it will almost certainly not cover all your living expenses, as studying must be the main emphasis, according to the law. There are labor laws that precisely stipulate how many hours students are allowed to work. The regulations vary, depending on where a student comes from.
+Are you a citizen of the EU, Iceland, Norway or Switzerland? You may work as much as you like without any additional permit. However, like German students, you should not work more than 20 hours a week during the semester. If you do, you will have to pay into social security
+Are you a citizen from a country not listed above? You are only allowed to work 120 full days or 240 half-days a year. Those who wish to work longer require a work permit from the Federal Employment Agency and the Aliens Registration Office (Ausländerbehörde). Whether you are issued a work permit largely depends on the conditions in the job market.</t>
+  </si>
+  <si>
+    <t>Academic performance is assigned a grade (mark) on a scale from 1.0 to 5.0, with 1.0 being “excellent” and 5.0 being a failing grade.
+Usually, credit points are awarded in accordance with the European Credit Transfer System (ECTS). The number of credit points depends on the workload of a specific course, not on the student’s performance in an examination. The workload reflects all the time and effort involved in attending a lecture or contributing to a seminar, including preparation and follow-up work, presentations and written work, as well as studying for tests or examinations.
+One credit point is deemed to be the equivalent of 25 – 30 working hours. The degree programs are usually structured so that students have to complete 30 credits per semester in order to complete the program in the prescribed time.</t>
+  </si>
+  <si>
+    <t>What facilities are there on campus?</t>
+  </si>
+  <si>
+    <t>Main Campus
+Ludwig-Guttmann-Str. 6 &amp; Maria-Probst-Str. 3
+Rektorat (Office of the Rector) 
+Arc 202. 
+Phone: +49 6221 88 2829
+Central Student Services
+Arc 102. 
+Phone: +49 6221 88 1000
+Academic Library 
+Bonhoeffer Str. 9 
+Phone: +49 6221 8223 285
+Opening hours: 24/7
+Cafeteria in the FORUM
+Phone: +49 6221 88 22 12 
+Opening hours: Monday-Thursday 8 a.m.-6.p.m., Friday 8 a.m.-4 p.m.</t>
+  </si>
+  <si>
+    <t>Rent a Bike</t>
+  </si>
+  <si>
+    <t>Where i can get a bike?</t>
+  </si>
+  <si>
+    <t>Used bicycles and rent-a-bike: 
+Radholz, Bergheimer Str. 101 or 
+Alte Eppelheimer Str. 31a, www.fahrrad-heidelberg.de</t>
+  </si>
+  <si>
+    <t>Which should i need to provided?</t>
+  </si>
+  <si>
+    <t>Detailed information about visa for Germany can be found on the websites of the German Federal Foreign Office.
+The entire visa procedure can take eight to twelve weeks, especially for fall intake, so ideally, you should submit your application for a visa as soon as you have the letter of admission from SRH University Heidelberg</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>Which type of Visa do i need?</t>
+  </si>
+  <si>
+    <t>As there are several types of visa, be sure to apply for a student visa, and under no circumstances come to Germany on a tourist visa. You cannot study in Germany on a tourist visa, and a tourist visa cannot be converted to a student visa.
+Student visas are usually issued for a three-month period. After you have arrived in Heidelberg and enrolled at SRH University Heidelberg, you will have to apply for an extended residence permit at the Aliens Registration Office in your town of residence (Heidelberg, Mannheim, Eppelheim, Schriesheim, etc).</t>
+  </si>
+  <si>
+    <t>Accomodations</t>
+  </si>
+  <si>
+    <t>Dorms on Campus</t>
+  </si>
+  <si>
+    <t>There are several dorms on campus, furnished with a bed, mattress, desk, chair, bookshelf, and wardrobe. Some have private bathrooms and some have shared kitchens. Please bring bedding and pillows with you or buy it at the International Office.</t>
+  </si>
+  <si>
+    <t>Health Insurance</t>
+  </si>
+  <si>
+    <t>As a student in Germany, you are required to have health insurance. Without proof of coverage, no German university will accept you.
+During Orientation Sessions we will have representatives at the university from German public health insurances. They will check your current insurance and advice.</t>
+  </si>
+  <si>
+    <t>Which Health Insurance do i need?</t>
+  </si>
+  <si>
+    <t>Application Documents</t>
+  </si>
+  <si>
+    <t>Which documents should i need to send with my application?</t>
+  </si>
+  <si>
+    <t>Please submit your application online to check your eligibility, attaching the following documents:
+University Entrance Qualification or Entrance Qualification for Universities of Applied Sciences (for Bachelor degree courses). Check the DAAD online admission database or Anabin to see whether your secondary school leaving certificate is recognized as a qualification for direct university admission in Germany.
+Bachelor certificate (for Master degree courses)
+Curriculum Vitae with current photo
+Certificate of a language proficiency (IELTS, TOEFL, Test DaF or similar) unless entrance qualifications were taken in English or German.
+Please note: you do NOT have to send us the application documents via post after you have completed the online application.</t>
+  </si>
+  <si>
+    <t>Language requirements</t>
+  </si>
+  <si>
+    <t>Do i need a Language Certificate?</t>
+  </si>
+  <si>
+    <t>For most degree programs, the language of instruction is German. You will therefore have to prove that you have an adequate knowledge of German. Applicants for a degree course need to have German language skills at level C1 of the Common European Framework of Reference for Languages.
+International degree programs taught in English require proof of language skills in English (for example, TOEFL, the “Test of English as a foreign language”). SRH University Heidelberg requires a minimum TOEFL score of 80 IBT, IELTS 6.0. Some programs may require a higher score, please check with the department in question.
+You are not required to have German language skills if your course of study is in English.</t>
+  </si>
+  <si>
+    <t>Mandatory Orientation Session</t>
+  </si>
+  <si>
+    <t>The International Office will organize Orientation during your first week, provide social and cultural advice, and link you up with other international students. And we will always be happy to assist you with formalities or any problems you may encounter.</t>
+  </si>
+  <si>
+    <t>When is the Orientation Session?</t>
+  </si>
+  <si>
+    <t>How much cost the semestrer Ticket?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heidelberg has an excellent local public transportation system, which students can ride inexpensively (€ 158,50) using the Semesterticket. </t>
+  </si>
+  <si>
+    <t>How long i can use the semester Ticket?</t>
+  </si>
+  <si>
+    <t>It is valid for 6 months</t>
+  </si>
+  <si>
+    <t>Maria-Probst-Str.3, at the main train station or online (text only in German!) as soon as you have enrolled.</t>
+  </si>
+  <si>
+    <t>Where i can get my semester ticket?</t>
+  </si>
+  <si>
+    <t>Semester Ticket</t>
+  </si>
+  <si>
+    <t>In Germany, all residents and visitors staying for longer than three months must register with the authorities. Once you have found accommodation, you have to inform the Residents’ Registration Office of your place of residence within one week.
+Students who live on campus have to go to the Residents’ Registration Office in Heidelberg-Wieblingen, Mannheimer Str. 259, and fill in a registration form (Anmeldebescheinigung).</t>
+  </si>
+  <si>
+    <t>Do i need a to register with the German Registration Office?</t>
+  </si>
+  <si>
+    <t>Residents’ Registration Office (Bürgerbüro)</t>
+  </si>
+  <si>
+    <t>Our university provides a MS Office Student Edition for each student. 
+Please go to this link and follow the steps described.</t>
+  </si>
+  <si>
+    <t>Does the Library make the full text of books available on the Website?</t>
+  </si>
+  <si>
+    <t>Only a small percentage of the total number of books in the Library's physical collections have been digitized or are available electronically through its website. 
+The bulk of digitized books available through the Library consist of approximately 136,000 books from the General Collections scanned by the Internet Archive, though several thousand additional titles have been scanned as a part of other projects and services.</t>
+  </si>
+  <si>
+    <t>How do I access electronic resources on and off campus?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using your SRH Credentials, you can access electronic resources from any computer—on or off of campus. All libraries provide unrestricted access to e-resources from public library computers located on campus.  </t>
+  </si>
+  <si>
+    <t>Ebooks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access </t>
+  </si>
+  <si>
+    <t>How do I borrow and renew materials?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To borrow items from SRH Library, take them with your ID to the appropriate circulation desk, and the staff will check them out to you. A growing number of libraries have self-checkout kiosks where you can checkout books as long as you have your ID card.  </t>
+  </si>
+  <si>
+    <t>Borrowing</t>
+  </si>
+  <si>
+    <t>Are SRHs libraries open to the public?</t>
+  </si>
+  <si>
+    <t>Yes they are open to the public, after 17.00 you need your id to stay in the library</t>
+  </si>
+  <si>
+    <t>I can’t find the answer to my question in these FAQ – where can I get more help?</t>
+  </si>
+  <si>
+    <t>Try Ask a Librarian for library and research-related questions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +470,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,9 +508,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,64 +856,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="71.44140625" customWidth="1"/>
-    <col min="4" max="4" width="77.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="315" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
+      <c r="C13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -626,17 +1265,17 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="8" max="8" width="31.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -644,42 +1283,42 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -691,27 +1330,27 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -723,13 +1362,13 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -742,16 +1381,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="88.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="88.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -759,7 +1398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -767,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -775,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -783,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -791,7 +1430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -813,30 +1452,30 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -852,33 +1491,33 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -894,46 +1533,46 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -949,29 +1588,29 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -987,34 +1626,34 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>